<commit_message>
Add project agent guidelines and update schemas
</commit_message>
<xml_diff>
--- a/ExternalTestData/Excel/MultiSheet.xlsx
+++ b/ExternalTestData/Excel/MultiSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CS Project\ExcelBinder\ExternalTestData\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C3FA7B3-4CD5-48B9-959A-E992F6265B38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78B0852A-0F2A-4089-A29B-0198F31C6877}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1905" yWindow="2580" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31050" yWindow="2925" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Item" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="8">
   <si>
     <t>Id</t>
   </si>
@@ -430,7 +430,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD3"/>
     </sheetView>
   </sheetViews>
@@ -489,9 +489,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.375" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -502,33 +504,23 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="A3">
         <v>1</v>
       </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="C5">
+      <c r="C3">
         <v>50</v>
       </c>
     </row>

</xml_diff>